<commit_message>
Fixes component list match (we have perfect match)
</commit_message>
<xml_diff>
--- a/sch/components.xlsx
+++ b/sch/components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miha\Desktop\vezje-idp\kicad\sch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66667DF9-155D-4464-A506-328CD4800B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7835F9-2275-499B-89E0-5C8DAB8BD279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{6172FD7F-16CD-47D1-A3E4-D63AC8EC044E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="428">
   <si>
     <t>ID</t>
   </si>
@@ -1086,9 +1086,6 @@
     <t>S14</t>
   </si>
   <si>
-    <t>C74</t>
-  </si>
-  <si>
     <t>S367</t>
   </si>
   <si>
@@ -1125,9 +1122,6 @@
     <t>33R</t>
   </si>
   <si>
-    <t>LS74</t>
-  </si>
-  <si>
     <t>MC14411</t>
   </si>
   <si>
@@ -1146,24 +1140,12 @@
     <t>4K7</t>
   </si>
   <si>
-    <t>P4?</t>
-  </si>
-  <si>
-    <t>P2?</t>
-  </si>
-  <si>
     <t>P1</t>
   </si>
   <si>
     <t>4.7K</t>
   </si>
   <si>
-    <t>4K7?</t>
-  </si>
-  <si>
-    <t>Z80CTC</t>
-  </si>
-  <si>
     <t>S20</t>
   </si>
   <si>
@@ -1215,9 +1197,6 @@
     <t>S38</t>
   </si>
   <si>
-    <t>S629?</t>
-  </si>
-  <si>
     <t>S393</t>
   </si>
   <si>
@@ -1260,9 +1239,6 @@
     <t>Z80 PIO (MK 3881)</t>
   </si>
   <si>
-    <t>P3 / S04</t>
-  </si>
-  <si>
     <t>2n 2 (?)</t>
   </si>
   <si>
@@ -1300,6 +1276,39 @@
   </si>
   <si>
     <t>390pF</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>S629</t>
+  </si>
+  <si>
+    <t>Z80 CTC</t>
+  </si>
+  <si>
+    <t>LS74 / S74</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Read as black-brown-red. Most likely it is green-brown-red (5K1).</t>
+  </si>
+  <si>
+    <t>"E75" (pg. 7)</t>
+  </si>
+  <si>
+    <t>Value Ref3</t>
+  </si>
+  <si>
+    <t>MM2716Q (EPROM)</t>
   </si>
 </sst>
 </file>
@@ -1354,11 +1363,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1673,20 +1682,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A507EC0B-FECA-46C5-861D-53A4B99CDA9D}">
-  <dimension ref="A1:G283"/>
+  <dimension ref="A1:I283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
-      <selection activeCell="B243" sqref="B243"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="G104" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="3" max="3" width="15.83984375" customWidth="1"/>
     <col min="4" max="4" width="15.5234375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.20703125" customWidth="1"/>
+    <col min="7" max="7" width="31.3125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.15625" customWidth="1"/>
+    <col min="9" max="9" width="53.9453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>343</v>
       </c>
@@ -1708,8 +1719,14 @@
       <c r="G1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H1" t="s">
+        <v>426</v>
+      </c>
+      <c r="I1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>79</v>
       </c>
@@ -1720,7 +1737,7 @@
         <v>77</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1729,11 +1746,11 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>71</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>70</v>
       </c>
       <c r="E3">
@@ -1743,7 +1760,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>96</v>
       </c>
@@ -1760,7 +1777,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>104</v>
       </c>
@@ -1777,7 +1794,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>199</v>
       </c>
@@ -1794,7 +1811,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>121</v>
       </c>
@@ -1805,7 +1822,7 @@
         <v>118</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1814,7 +1831,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>75</v>
       </c>
@@ -1825,7 +1842,7 @@
         <v>73</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1834,7 +1851,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>97</v>
       </c>
@@ -1851,7 +1868,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>83</v>
       </c>
@@ -1862,7 +1879,7 @@
         <v>81</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -1871,7 +1888,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>98</v>
       </c>
@@ -1888,7 +1905,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>99</v>
       </c>
@@ -1905,7 +1922,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>100</v>
       </c>
@@ -1922,7 +1939,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>101</v>
       </c>
@@ -1939,7 +1956,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>102</v>
       </c>
@@ -1956,7 +1973,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>174</v>
       </c>
@@ -1967,7 +1984,7 @@
         <v>168</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1987,7 +2004,7 @@
         <v>169</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -2017,7 +2034,7 @@
       <c r="A19">
         <v>72</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E19">
@@ -2038,7 +2055,7 @@
         <v>239</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -2058,7 +2075,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -2081,7 +2098,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -2097,7 +2114,7 @@
       <c r="A23">
         <v>61</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E23">
@@ -2118,7 +2135,7 @@
         <v>10</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -2141,7 +2158,7 @@
         <v>242</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -2154,7 +2171,7 @@
       <c r="A26">
         <v>62</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E26">
@@ -2175,7 +2192,7 @@
         <v>51</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -2195,7 +2212,7 @@
         <v>40</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -2215,7 +2232,7 @@
         <v>38</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -2235,7 +2252,7 @@
         <v>39</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -2265,7 +2282,7 @@
       <c r="A32">
         <v>1</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E32">
@@ -2282,7 +2299,7 @@
       <c r="A33">
         <v>15</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E33">
@@ -2299,7 +2316,7 @@
       <c r="A34">
         <v>24</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E34">
@@ -2316,7 +2333,7 @@
       <c r="A35">
         <v>48</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E35">
@@ -2333,7 +2350,7 @@
       <c r="A36">
         <v>74</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E36">
@@ -2350,7 +2367,7 @@
       <c r="A37">
         <v>108</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E37">
@@ -2367,7 +2384,7 @@
       <c r="A38">
         <v>125</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E38">
@@ -2384,7 +2401,7 @@
       <c r="A39">
         <v>130</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E39">
@@ -2401,7 +2418,7 @@
       <c r="A40">
         <v>144</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E40">
@@ -2418,7 +2435,7 @@
       <c r="A41">
         <v>163</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E41">
@@ -2435,7 +2452,7 @@
       <c r="A42">
         <v>186</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E42">
@@ -2452,7 +2469,7 @@
       <c r="A43">
         <v>195</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E43">
@@ -2469,7 +2486,7 @@
       <c r="A44">
         <v>213</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E44">
@@ -2486,7 +2503,7 @@
       <c r="A45">
         <v>221</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E45">
@@ -2503,7 +2520,7 @@
       <c r="A46">
         <v>248</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E46">
@@ -2520,7 +2537,7 @@
       <c r="A47">
         <v>264</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E47">
@@ -2567,7 +2584,7 @@
         <v>6</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -2636,7 +2653,7 @@
         <v>254</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -2659,7 +2676,7 @@
         <v>247</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -2682,7 +2699,7 @@
         <v>248</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -2705,7 +2722,7 @@
         <v>249</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -2728,7 +2745,7 @@
         <v>250</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -2751,7 +2768,7 @@
         <v>251</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -2774,7 +2791,7 @@
         <v>252</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -2797,7 +2814,7 @@
         <v>7</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -2820,7 +2837,7 @@
         <v>57</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -2843,7 +2860,7 @@
         <v>58</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -2866,7 +2883,7 @@
         <v>49</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -2889,7 +2906,7 @@
         <v>48</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -2912,7 +2929,7 @@
         <v>29</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -2935,7 +2952,7 @@
         <v>30</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -2958,7 +2975,7 @@
         <v>31</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -2981,7 +2998,7 @@
         <v>22</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -3027,7 +3044,7 @@
         <v>23</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -3050,7 +3067,7 @@
         <v>24</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -3073,7 +3090,7 @@
         <v>8</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -3096,7 +3113,7 @@
         <v>9</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -3119,7 +3136,7 @@
         <v>15</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E73">
         <v>1</v>
@@ -3142,7 +3159,7 @@
         <v>16</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E74">
         <v>1</v>
@@ -3165,7 +3182,7 @@
         <v>120</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -3188,7 +3205,7 @@
         <v>121</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -3211,7 +3228,7 @@
         <v>119</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -3234,7 +3251,7 @@
         <v>110</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E78">
         <v>1</v>
@@ -3256,8 +3273,8 @@
       <c r="C79" t="s">
         <v>41</v>
       </c>
-      <c r="D79" s="3" t="s">
-        <v>353</v>
+      <c r="D79" s="2" t="s">
+        <v>360</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -3280,7 +3297,7 @@
         <v>106</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -3303,7 +3320,7 @@
         <v>107</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -3326,7 +3343,7 @@
         <v>108</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -3349,7 +3366,7 @@
         <v>109</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="E83">
         <v>1</v>
@@ -3372,7 +3389,7 @@
         <v>92</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E84">
         <v>1</v>
@@ -3395,7 +3412,7 @@
         <v>91</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="E85">
         <v>1</v>
@@ -3418,7 +3435,7 @@
         <v>74</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E86">
         <v>1</v>
@@ -3441,7 +3458,7 @@
         <v>101</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E87">
         <v>1</v>
@@ -3464,7 +3481,7 @@
         <v>75</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E88">
         <v>1</v>
@@ -3487,7 +3504,7 @@
         <v>82</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E89">
         <v>1</v>
@@ -3533,7 +3550,7 @@
         <v>80</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="E91">
         <v>1</v>
@@ -3556,7 +3573,7 @@
         <v>76</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E92">
         <v>1</v>
@@ -3657,7 +3674,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A97">
         <v>136</v>
       </c>
@@ -3668,7 +3685,7 @@
         <v>132</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E97">
         <v>1</v>
@@ -3680,7 +3697,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A98">
         <v>137</v>
       </c>
@@ -3691,7 +3708,7 @@
         <v>133</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E98">
         <v>1</v>
@@ -3703,7 +3720,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A99">
         <v>129</v>
       </c>
@@ -3714,7 +3731,7 @@
         <v>126</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="E99">
         <v>1</v>
@@ -3726,7 +3743,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A100">
         <v>126</v>
       </c>
@@ -3737,7 +3754,7 @@
         <v>122</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="E100">
         <v>1</v>
@@ -3749,7 +3766,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A101">
         <v>26</v>
       </c>
@@ -3760,7 +3777,7 @@
         <v>26</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -3772,7 +3789,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A102">
         <v>127</v>
       </c>
@@ -3782,7 +3799,7 @@
       <c r="C102" t="s">
         <v>123</v>
       </c>
-      <c r="D102" s="2">
+      <c r="D102" s="5">
         <v>2716</v>
       </c>
       <c r="E102">
@@ -3795,7 +3812,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A103">
         <v>128</v>
       </c>
@@ -3805,7 +3822,7 @@
       <c r="C103" t="s">
         <v>124</v>
       </c>
-      <c r="D103" s="2">
+      <c r="D103" s="5">
         <v>2716</v>
       </c>
       <c r="E103">
@@ -3815,10 +3832,13 @@
         <v>3.1</v>
       </c>
       <c r="G103" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>279</v>
+      </c>
+      <c r="H103" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A104">
         <v>141</v>
       </c>
@@ -3841,7 +3861,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A105">
         <v>134</v>
       </c>
@@ -3864,7 +3884,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A106">
         <v>133</v>
       </c>
@@ -3875,7 +3895,7 @@
         <v>129</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E106">
         <v>1</v>
@@ -3887,7 +3907,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A107">
         <v>132</v>
       </c>
@@ -3898,7 +3918,7 @@
         <v>128</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="E107">
         <v>1</v>
@@ -3910,7 +3930,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A108">
         <v>131</v>
       </c>
@@ -3933,7 +3953,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A109">
         <v>172</v>
       </c>
@@ -3944,7 +3964,7 @@
         <v>166</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="E109">
         <v>1</v>
@@ -3956,7 +3976,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A110">
         <v>173</v>
       </c>
@@ -3979,7 +3999,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A111">
         <v>145</v>
       </c>
@@ -4002,7 +4022,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A112">
         <v>27</v>
       </c>
@@ -4013,7 +4033,7 @@
         <v>27</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E112">
         <v>1</v>
@@ -4105,7 +4125,7 @@
         <v>177</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="E116">
         <v>1</v>
@@ -4128,7 +4148,7 @@
         <v>175</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E117">
         <v>1</v>
@@ -4151,7 +4171,7 @@
         <v>161</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="E118">
         <v>1</v>
@@ -4174,7 +4194,7 @@
         <v>162</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E119">
         <v>1</v>
@@ -4197,7 +4217,7 @@
         <v>163</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>378</v>
+        <v>421</v>
       </c>
       <c r="E120">
         <v>1</v>
@@ -4220,7 +4240,7 @@
         <v>164</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E121">
         <v>1</v>
@@ -4243,7 +4263,7 @@
         <v>165</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E122">
         <v>1</v>
@@ -4266,7 +4286,7 @@
         <v>17</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E123">
         <v>1</v>
@@ -4289,7 +4309,7 @@
         <v>171</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>396</v>
+        <v>420</v>
       </c>
       <c r="E124">
         <v>1</v>
@@ -4404,7 +4424,7 @@
         <v>218</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="E129">
         <v>1</v>
@@ -4427,7 +4447,7 @@
         <v>215</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="E130">
         <v>1</v>
@@ -4450,7 +4470,7 @@
         <v>205</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E131">
         <v>1</v>
@@ -4473,7 +4493,7 @@
         <v>206</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="E132">
         <v>1</v>
@@ -4496,7 +4516,7 @@
         <v>207</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="E133">
         <v>1</v>
@@ -4519,7 +4539,7 @@
         <v>18</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E134">
         <v>1</v>
@@ -4539,10 +4559,10 @@
         <v>208</v>
       </c>
       <c r="C135" t="s">
-        <v>201</v>
+        <v>425</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>394</v>
+        <v>355</v>
       </c>
       <c r="E135">
         <v>1</v>
@@ -4562,10 +4582,10 @@
         <v>201</v>
       </c>
       <c r="C136" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>356</v>
+        <v>388</v>
       </c>
       <c r="E136">
         <v>1</v>
@@ -4585,10 +4605,10 @@
         <v>199</v>
       </c>
       <c r="C137" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
       <c r="E137">
         <v>1</v>
@@ -4611,7 +4631,7 @@
         <v>193</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>361</v>
+        <v>422</v>
       </c>
       <c r="E138">
         <v>1</v>
@@ -4634,7 +4654,7 @@
         <v>203</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E139">
         <v>1</v>
@@ -4749,7 +4769,7 @@
         <v>219</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>373</v>
+        <v>419</v>
       </c>
       <c r="E144">
         <v>1</v>
@@ -4772,7 +4792,7 @@
         <v>19</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="E145">
         <v>1</v>
@@ -4795,7 +4815,7 @@
         <v>216</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>374</v>
+        <v>418</v>
       </c>
       <c r="E146">
         <v>1</v>
@@ -4818,7 +4838,7 @@
         <v>209</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E147">
         <v>1</v>
@@ -4841,7 +4861,7 @@
         <v>210</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="E148">
         <v>1</v>
@@ -4864,7 +4884,7 @@
         <v>211</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="E149">
         <v>1</v>
@@ -4887,7 +4907,7 @@
         <v>202</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E150">
         <v>1</v>
@@ -4933,7 +4953,7 @@
         <v>197</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="E152">
         <v>1</v>
@@ -4956,7 +4976,7 @@
         <v>194</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="E153">
         <v>1</v>
@@ -5450,7 +5470,7 @@
         <v>62</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E181">
         <v>1</v>
@@ -5473,7 +5493,7 @@
         <v>50</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="E182">
         <v>1</v>
@@ -5513,7 +5533,7 @@
         <v>47</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E184">
         <v>1</v>
@@ -5533,7 +5553,7 @@
         <v>46</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E185">
         <v>1</v>
@@ -5573,7 +5593,7 @@
         <v>44</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E187">
         <v>1</v>
@@ -5593,7 +5613,7 @@
         <v>43</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E188">
         <v>1</v>
@@ -5636,7 +5656,7 @@
         <v>33</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E190">
         <v>1</v>
@@ -5682,7 +5702,7 @@
         <v>63</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E192">
         <v>1</v>
@@ -5728,7 +5748,7 @@
         <v>104</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="E194">
         <v>1</v>
@@ -5748,7 +5768,7 @@
         <v>105</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="E195">
         <v>1</v>
@@ -5768,7 +5788,7 @@
         <v>159</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E196">
         <v>1</v>
@@ -5834,7 +5854,7 @@
         <v>21</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="E199">
         <v>1</v>
@@ -5857,7 +5877,7 @@
         <v>4</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E200">
         <v>1</v>
@@ -5877,10 +5897,10 @@
         <v>5</v>
       </c>
       <c r="C201" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E201">
         <v>1</v>
@@ -5903,7 +5923,7 @@
         <v>14</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="E202">
         <v>1</v>
@@ -5960,7 +5980,7 @@
         <v>64</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E205">
         <v>1</v>
@@ -6085,7 +6105,7 @@
         <v>103</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E212">
         <v>1</v>
@@ -6165,7 +6185,7 @@
         <v>65</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E216">
         <v>1</v>
@@ -6248,7 +6268,7 @@
         <v>148</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E220">
         <v>1</v>
@@ -6271,7 +6291,7 @@
         <v>149</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E221">
         <v>1</v>
@@ -6294,7 +6314,7 @@
         <v>150</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E222">
         <v>1</v>
@@ -6317,7 +6337,7 @@
         <v>151</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E223">
         <v>1</v>
@@ -6340,7 +6360,7 @@
         <v>152</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E224">
         <v>1</v>
@@ -6352,7 +6372,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A225">
         <v>158</v>
       </c>
@@ -6363,7 +6383,7 @@
         <v>153</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E225">
         <v>1</v>
@@ -6375,7 +6395,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A226">
         <v>159</v>
       </c>
@@ -6386,7 +6406,7 @@
         <v>154</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E226">
         <v>1</v>
@@ -6398,7 +6418,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A227">
         <v>67</v>
       </c>
@@ -6409,7 +6429,7 @@
         <v>66</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E227">
         <v>1</v>
@@ -6421,7 +6441,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A228">
         <v>160</v>
       </c>
@@ -6432,7 +6452,7 @@
         <v>155</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E228">
         <v>1</v>
@@ -6444,7 +6464,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A229">
         <v>161</v>
       </c>
@@ -6455,7 +6475,7 @@
         <v>156</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E229">
         <v>1</v>
@@ -6467,7 +6487,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A230">
         <v>162</v>
       </c>
@@ -6478,7 +6498,7 @@
         <v>157</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E230">
         <v>1</v>
@@ -6490,7 +6510,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A231">
         <v>176</v>
       </c>
@@ -6501,7 +6521,7 @@
         <v>170</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="E231">
         <v>1</v>
@@ -6512,8 +6532,11 @@
       <c r="G231" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="I231" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A232">
         <v>196</v>
       </c>
@@ -6524,7 +6547,7 @@
         <v>188</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E232">
         <v>1</v>
@@ -6536,7 +6559,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A233">
         <v>200</v>
       </c>
@@ -6547,7 +6570,7 @@
         <v>192</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E233">
         <v>1</v>
@@ -6559,7 +6582,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A234">
         <v>204</v>
       </c>
@@ -6576,7 +6599,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A235">
         <v>207</v>
       </c>
@@ -6593,7 +6616,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A236">
         <v>178</v>
       </c>
@@ -6604,7 +6627,7 @@
         <v>172</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E236">
         <v>1</v>
@@ -6616,7 +6639,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A237">
         <v>179</v>
       </c>
@@ -6627,7 +6650,7 @@
         <v>173</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E237">
         <v>1</v>
@@ -6639,7 +6662,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A238">
         <v>230</v>
       </c>
@@ -6650,7 +6673,7 @@
         <v>220</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E238">
         <v>1</v>
@@ -6662,7 +6685,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A239">
         <v>231</v>
       </c>
@@ -6673,7 +6696,7 @@
         <v>221</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E239">
         <v>1</v>
@@ -6685,7 +6708,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A240">
         <v>232</v>
       </c>
@@ -6696,7 +6719,7 @@
         <v>222</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E240">
         <v>1</v>
@@ -6719,7 +6742,7 @@
         <v>223</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E241">
         <v>1</v>
@@ -6742,7 +6765,7 @@
         <v>224</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E242">
         <v>1</v>
@@ -6758,14 +6781,14 @@
       <c r="A243">
         <v>235</v>
       </c>
-      <c r="B243" s="5" t="s">
+      <c r="B243" s="4" t="s">
         <v>225</v>
       </c>
       <c r="C243" t="s">
         <v>225</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E243">
         <v>1</v>
@@ -6788,7 +6811,7 @@
         <v>226</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E244">
         <v>1</v>
@@ -6811,7 +6834,7 @@
         <v>227</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E245">
         <v>1</v>
@@ -6834,7 +6857,7 @@
         <v>228</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E246">
         <v>1</v>
@@ -6857,7 +6880,7 @@
         <v>229</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E247">
         <v>1</v>
@@ -6880,7 +6903,7 @@
         <v>67</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E248">
         <v>1</v>
@@ -6903,7 +6926,7 @@
         <v>230</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E249">
         <v>1</v>
@@ -6926,7 +6949,7 @@
         <v>231</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E250">
         <v>1</v>
@@ -6949,7 +6972,7 @@
         <v>232</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E251">
         <v>1</v>
@@ -6972,7 +6995,7 @@
         <v>233</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E252">
         <v>1</v>
@@ -6995,7 +7018,7 @@
         <v>234</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E253">
         <v>1</v>
@@ -7018,7 +7041,7 @@
         <v>235</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E254">
         <v>1</v>
@@ -7041,7 +7064,7 @@
         <v>236</v>
       </c>
       <c r="D255" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E255">
         <v>1</v>
@@ -7064,7 +7087,7 @@
         <v>237</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E256">
         <v>1</v>
@@ -7087,7 +7110,7 @@
         <v>256</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E257">
         <v>1</v>
@@ -7110,7 +7133,7 @@
         <v>257</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="E258">
         <v>1</v>
@@ -7133,7 +7156,7 @@
         <v>258</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="E259">
         <v>1</v>
@@ -7156,7 +7179,7 @@
         <v>259</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E260">
         <v>1</v>
@@ -7179,7 +7202,7 @@
         <v>260</v>
       </c>
       <c r="D261" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E261">
         <v>1</v>
@@ -7202,7 +7225,7 @@
         <v>261</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E262">
         <v>1</v>
@@ -7225,7 +7248,7 @@
         <v>262</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E263">
         <v>1</v>
@@ -7248,7 +7271,7 @@
         <v>263</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E264">
         <v>1</v>
@@ -7271,7 +7294,7 @@
         <v>213</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E265">
         <v>1</v>
@@ -7291,7 +7314,7 @@
         <v>240</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="E266">
         <v>1</v>
@@ -7314,7 +7337,7 @@
         <v>241</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="E267">
         <v>1</v>
@@ -7337,7 +7360,7 @@
         <v>243</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="E268">
         <v>1</v>
@@ -7357,7 +7380,7 @@
         <v>68</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E269">
         <v>1</v>
@@ -7403,7 +7426,7 @@
         <v>217</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E271">
         <v>1</v>
@@ -7426,7 +7449,7 @@
         <v>189</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="E272">
         <v>1</v>
@@ -7449,7 +7472,7 @@
         <v>190</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="E273">
         <v>1</v>
@@ -7555,7 +7578,7 @@
         <v>78</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="E278">
         <v>1</v>
@@ -7575,7 +7598,7 @@
         <v>79</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="E279">
         <v>1</v>
@@ -7636,7 +7659,7 @@
         <v>11</v>
       </c>
       <c r="D282" s="2" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="E282">
         <v>1</v>
@@ -7659,7 +7682,7 @@
         <v>158</v>
       </c>
       <c r="D283" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E283">
         <v>1</v>

</xml_diff>